<commit_message>
Update Category & Book Controller
</commit_message>
<xml_diff>
--- a/HaT7FptBook/wwwroot/Uploads/CategoriList.xlsx
+++ b/HaT7FptBook/wwwroot/Uploads/CategoriList.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nguyenminhtri/Desktop/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2D310078-82D8-4946-BB23-215BA5C096A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="5160" yWindow="1780" windowWidth="28040" windowHeight="17440" xr2:uid="{6E4F188E-9595-F442-A3DF-4FCABB0B8541}"/>
+    <workbookView xWindow="5160" yWindow="1776" windowWidth="23256" windowHeight="13176"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -58,7 +52,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -150,7 +144,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -202,7 +196,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -396,23 +390,23 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB3E80D7-38BC-C946-B748-E0E1D29CD45F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="283" workbookViewId="0">
-      <selection sqref="A1:B3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -420,7 +414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -428,7 +422,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>

</xml_diff>